<commit_message>
Visualizer last version and Basel document.
</commit_message>
<xml_diff>
--- a/Documentation/Classification.xlsx
+++ b/Documentation/Classification.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14600" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="____init___" sheetId="14" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="99">
   <si>
     <t>Dodd-Frank XML document</t>
   </si>
@@ -330,6 +330,9 @@
   </si>
   <si>
     <t>Mail Config</t>
+  </si>
+  <si>
+    <t>Javascript is inside of the Login.html</t>
   </si>
 </sst>
 </file>
@@ -2842,8 +2845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3290,10 +3293,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3303,27 +3306,27 @@
     <col min="12" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D1" s="14" t="s">
         <v>65</v>
       </c>
       <c r="E1" s="15"/>
     </row>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.2">
       <c r="G2" s="16" t="s">
         <v>64</v>
       </c>
       <c r="H2" s="17"/>
     </row>
-    <row r="3" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="G3" s="18"/>
       <c r="H3" s="19"/>
     </row>
-    <row r="5" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="G5" s="20"/>
       <c r="H5" s="20"/>
     </row>
-    <row r="6" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D6" s="21" t="s">
         <v>64</v>
       </c>
@@ -3336,15 +3339,18 @@
         <v>67</v>
       </c>
       <c r="K6" s="22"/>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="N6" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>61</v>
       </c>
       <c r="G7" s="26"/>
       <c r="H7" s="26"/>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.2">
       <c r="D9" s="2" t="s">
         <v>68</v>
       </c>
@@ -3359,8 +3365,8 @@
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D13" s="23" t="s">
         <v>71</v>
       </c>
@@ -3372,10 +3378,10 @@
       <c r="J13" s="24"/>
       <c r="K13" s="25"/>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:14" x14ac:dyDescent="0.2">
       <c r="H14" s="6"/>
     </row>
-    <row r="16" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="17" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D17" s="21" t="s">
         <v>12</v>

</xml_diff>